<commit_message>
add form đh + tài liệu
</commit_message>
<xml_diff>
--- a/Tai lieu dd2/Bang diem lop 3 LTDD2.xlsx
+++ b/Tai lieu dd2/Bang diem lop 3 LTDD2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="108">
   <si>
     <t>Đề số</t>
   </si>
@@ -24,9 +24,6 @@
   </si>
   <si>
     <t>link github</t>
-  </si>
-  <si>
-    <t>EXE4</t>
   </si>
   <si>
     <t>EXE5</t>
@@ -296,11 +293,6 @@
     <t>17-31</t>
   </si>
   <si>
-    <t>EXE3
-- Bài 1: screen 4đ
-- Bài 2:  animation : 4 đ</t>
-  </si>
-  <si>
     <t>animation scale</t>
   </si>
   <si>
@@ -319,9 +311,6 @@
     <t>layout chat</t>
   </si>
   <si>
-    <t>media_layed</t>
-  </si>
-  <si>
     <t>20_37</t>
   </si>
   <si>
@@ -329,6 +318,53 @@
   </si>
   <si>
     <t>06-18</t>
+  </si>
+  <si>
+    <t>media_layer</t>
+  </si>
+  <si>
+    <t>record media</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>camera</t>
+  </si>
+  <si>
+    <t>15-20</t>
+  </si>
+  <si>
+    <t>6-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXE4: Danh sach, Chuc nang
+1. media player
+2. media Record
+3.Camera 
+4.call,  msg, </t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>smg</t>
+  </si>
+  <si>
+    <t>EXE3 : Đồ án
+- Drawable: 2 +2
+- animation: 2 +2
+- icon: (nhóm ):1
+- UI: -2</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>8-34</t>
   </si>
 </sst>
 </file>
@@ -344,7 +380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +390,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -412,6 +454,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,10 +761,10 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G36" sqref="G36:G37"/>
+      <selection pane="bottomRight" activeCell="H32" sqref="H32:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +775,8 @@
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -738,40 +784,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -779,17 +825,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="6">
         <v>6</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -804,17 +852,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="6">
         <v>4</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1">
+        <v>6</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -829,17 +879,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -858,7 +910,9 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -871,10 +925,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -898,10 +952,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -925,17 +979,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>6</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -950,17 +1006,19 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
         <v>6</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -975,10 +1033,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1002,10 +1060,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1029,17 +1087,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
         <v>7</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="11">
+        <v>7</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1054,17 +1114,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="6">
         <v>2</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1">
+        <v>7</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1079,10 +1141,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1106,10 +1168,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1133,10 +1195,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1146,7 +1208,9 @@
       <c r="G16" s="6">
         <v>8</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="6">
+        <v>5</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="3">
@@ -1160,10 +1224,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1173,7 +1237,9 @@
       <c r="G17" s="6">
         <v>8</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="6">
+        <v>5</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3">
@@ -1187,10 +1253,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1200,7 +1266,9 @@
       <c r="G18" s="6">
         <v>8</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="6">
+        <v>9</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="3">
@@ -1214,10 +1282,10 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1227,7 +1295,9 @@
       <c r="G19" s="6">
         <v>8</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="6">
+        <v>9</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="3">
@@ -1241,17 +1311,19 @@
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="6">
         <v>4</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="K20" s="1">
@@ -1265,17 +1337,19 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1">
         <v>3</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="K21" s="1">
@@ -1289,17 +1363,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="6">
         <v>6</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1">
+        <v>6</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1314,17 +1390,19 @@
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="6">
         <v>5</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1">
+        <v>6</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1339,17 +1417,19 @@
         <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="6">
         <v>7</v>
       </c>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1">
+        <v>7</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1364,17 +1444,19 @@
         <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="6">
         <v>7</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1">
+        <v>7</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1389,17 +1471,19 @@
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1">
         <v>4</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1">
+        <v>7</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1414,17 +1498,19 @@
         <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1">
         <v>4</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <v>7</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1439,17 +1525,19 @@
         <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1">
         <v>7</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <v>5</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1464,17 +1552,19 @@
         <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1">
         <v>7</v>
       </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1">
+        <v>5</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1489,17 +1579,19 @@
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="6">
         <v>2</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1">
+        <v>8</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1514,17 +1606,19 @@
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="6">
         <v>2</v>
       </c>
-      <c r="G31" s="1"/>
+      <c r="G31" s="1">
+        <v>8</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1539,18 +1633,22 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1">
         <v>5</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="G32" s="1">
+        <v>5</v>
+      </c>
+      <c r="H32" s="6">
+        <v>5</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="3">
@@ -1564,18 +1662,22 @@
         <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1">
         <v>5</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="G33" s="1">
+        <v>5</v>
+      </c>
+      <c r="H33" s="6">
+        <v>5</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="3">
@@ -1589,17 +1691,19 @@
         <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1">
         <v>0</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1614,17 +1718,19 @@
         <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1">
         <v>2</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35" s="1">
+        <v>4</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1639,10 +1745,10 @@
         <v>20</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1666,10 +1772,10 @@
         <v>20</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1693,11 +1799,11 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -1705,7 +1811,7 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -1713,7 +1819,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1726,10 +1832,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,24 +1845,24 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1769,7 +1875,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1782,7 +1888,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1">
         <v>9</v>
@@ -1793,7 +1899,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1">
         <v>9</v>
@@ -1806,7 +1912,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
@@ -1817,7 +1923,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="6">
         <v>4</v>
@@ -1830,16 +1936,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
@@ -1847,13 +1953,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -1862,13 +1968,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1877,13 +1983,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1892,13 +1998,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1907,10 +2013,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1920,10 +2026,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1933,39 +2039,196 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>